<commit_message>
ADDED: context canceling to parser, service_test, .env.example     UPDATE: README.MD
</commit_message>
<xml_diff>
--- a/test3.xlsx
+++ b/test3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d6d4ef9c8c8122a/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_AD4DF75460589B3ACB72842D1F5E43405BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6325A906-057C-4C0F-B30B-FE9172611588}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_AD4DF75460589B3ACB72842D1F5E43405BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CF430C5-8196-4848-80FA-BA3A0D5C9253}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="14460" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>salary</t>
   </si>
   <si>
-    <t>in russia</t>
-  </si>
-  <si>
     <t>Sasha</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>is_active</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +397,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -405,14 +405,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <f>12000 + 0.1</f>
         <v>12000.1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -420,14 +420,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <f>1000.15</f>
         <v>1000.15</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -435,13 +435,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>25000.5</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>